<commit_message>
Fix space error in CSV template
</commit_message>
<xml_diff>
--- a/csv/gatol_question_set_template.xlsx
+++ b/csv/gatol_question_set_template.xlsx
@@ -46,7 +46,7 @@
     <t>Wrong Answer 6</t>
   </si>
   <si>
-    <t>Wrong Answer7</t>
+    <t>Wrong Answer 7</t>
   </si>
 </sst>
 </file>
@@ -146,15 +146,15 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J:AMJ"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
     <col collapsed="false" hidden="true" max="1025" min="10" style="0" width="0"/>
   </cols>
   <sheetData>

</xml_diff>